<commit_message>
Database creation, 1st go
</commit_message>
<xml_diff>
--- a/database/data/school.xlsx
+++ b/database/data/school.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/Desktop/CS316/316_project/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/Desktop/CS316/316_project/database/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="620" windowWidth="24160" windowHeight="12960" tabRatio="500"/>
+    <workbookView xWindow="13840" yWindow="460" windowWidth="11760" windowHeight="12960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="school.csv" sheetId="1" r:id="rId1"/>
@@ -27,19 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Tuition</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Duke University</t>
   </si>
@@ -390,9 +378,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -404,134 +394,153 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="B1" s="1">
+        <v>6501</v>
+      </c>
+      <c r="C1" s="2">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1">
+        <v>63999</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>6501</v>
+        <v>16126</v>
+      </c>
+      <c r="C2" s="2">
+        <v>9</v>
       </c>
       <c r="D2" s="1">
-        <v>63999</v>
+        <v>19359</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>16126</v>
+        <v>1779</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>19359</v>
+        <v>60921</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1779</v>
+        <v>21697</v>
+      </c>
+      <c r="C4" s="2">
+        <v>207</v>
       </c>
       <c r="D4" s="1">
-        <v>60921</v>
+        <v>21040</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>21697</v>
+        <v>5903</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>21040</v>
+        <v>45186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>5903</v>
+        <v>4362</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>45186</v>
+        <v>46710</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>4362</v>
+        <v>17951</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30</v>
       </c>
       <c r="D7" s="1">
-        <v>46710</v>
+        <v>23940</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>17951</v>
+        <v>12971</v>
+      </c>
+      <c r="C8" s="2">
+        <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>23940</v>
+        <v>21050</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>12971</v>
+        <v>4866</v>
+      </c>
+      <c r="C9" s="2">
+        <v>27</v>
       </c>
       <c r="D9" s="1">
-        <v>21050</v>
+        <v>62502</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>4866</v>
+        <v>15158</v>
+      </c>
+      <c r="C10" s="2">
+        <v>198</v>
       </c>
       <c r="D10" s="1">
-        <v>62502</v>
+        <v>18357</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>15158</v>
+        <v>1551</v>
+      </c>
+      <c r="C11" s="2">
+        <v>20</v>
       </c>
       <c r="D11" s="1">
-        <v>18357</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1551</v>
-      </c>
-      <c r="D12" s="1">
         <v>46333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-Updated database files to include degree tables
</commit_message>
<xml_diff>
--- a/database/data/school.xlsx
+++ b/database/data/school.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -347,7 +347,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,7 +374,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,16 +654,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -689,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -703,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -717,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -731,21 +734,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
+        <v>4524</v>
+      </c>
+      <c r="C6" s="1">
         <v>49892</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4524</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -759,7 +762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -773,7 +776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -787,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -801,7 +804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -815,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -829,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -843,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -857,7 +860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -871,7 +874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -885,7 +888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -899,7 +902,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -913,7 +916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -927,7 +930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -941,7 +944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -955,7 +958,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -969,7 +972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -983,7 +986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1473,7 +1476,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1487,7 +1490,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -1515,7 +1518,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -1809,7 +1812,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -1865,7 +1868,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -1879,7 +1882,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -1935,7 +1938,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -1977,7 +1980,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
@@ -2047,7 +2050,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>

</xml_diff>